<commit_message>
Added LTE station code
</commit_message>
<xml_diff>
--- a/hardware/hardware_spreadsheet_campbellsci.xlsx
+++ b/hardware/hardware_spreadsheet_campbellsci.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braedon Dority\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braedon Dority\Documents\GitHub\snow_sensing\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{031CBC4C-D6A5-4DE6-83F3-1DC519B58C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5767319A-FB03-42F2-95CA-58E81E25D4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{6EB52CEB-1D4B-9D4B-8914-58F1C62D238A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
   <si>
     <t>Item</t>
   </si>
@@ -125,9 +125,6 @@
     <t xml:space="preserve">    U-bolts</t>
   </si>
   <si>
-    <t xml:space="preserve">    12V 10Ah Lead acid battery</t>
-  </si>
-  <si>
     <t xml:space="preserve">    CH150 12V charging regulator</t>
   </si>
   <si>
@@ -185,24 +182,15 @@
     <t>900 MHz - but other options available</t>
   </si>
   <si>
-    <t>32 GB (Link is to a pack of 2 for $11.15)</t>
-  </si>
-  <si>
     <t>Provides stereo sensor connectors (Sold in packs of 5 for $35.00)</t>
   </si>
   <si>
     <t>Cable for Maxbotix snow depth sensor (Price is per foot. Length depends on deployment platform).</t>
   </si>
   <si>
-    <t>For securing and connecting peripheral ADCs. Sold in packs of 5 for $11.99</t>
-  </si>
-  <si>
     <t>Necessary to expand Mayfly datalogger for taking differential measurements from all radiation sensors</t>
   </si>
   <si>
-    <t>Waterproof datalogger enclosure</t>
-  </si>
-  <si>
     <t>For fastening the enclosure to the mast. These are zinc plated. Stainless would be better but more expensive.</t>
   </si>
   <si>
@@ -221,24 +209,15 @@
     <t>For plugging the aluminum conduit - keeps out the critters</t>
   </si>
   <si>
-    <t>Sold in 100ft length at $99. Used for protecting soil moisture sensor cables from critters.</t>
-  </si>
-  <si>
     <t xml:space="preserve">    16.8V, 0.59 A, 10W solar panel with mounting bracket</t>
   </si>
   <si>
     <t>Power system needs to power a 12V battery - 12V power is needed to run internal heaters on Apogee sensors</t>
   </si>
   <si>
-    <t>Can find these cheaper online. This is local store price. Purchased two batteries so we can swap during site visits.</t>
-  </si>
-  <si>
     <t>We had these on hand so didn't buy new ones. You cand find cheaper charge regulators online.</t>
   </si>
   <si>
-    <t>Sold in package of 20 for $4.19. Termination on other end of battery power cable depends on charge regulator.</t>
-  </si>
-  <si>
     <t xml:space="preserve">    PVC Jacketed 22 Gauge 5 conductor wire - cabling for MaxBotix sensor</t>
   </si>
   <si>
@@ -260,21 +239,9 @@
     <t>Pulse width or single ended voltage output</t>
   </si>
   <si>
-    <t xml:space="preserve">    EnvrioDIY grove to 3.5mm stereo jack (pack of 5)</t>
-  </si>
-  <si>
     <t xml:space="preserve">    MicroSD card (pack of 2)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Compact wire splice connector quick terminal block (pack of 8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Prototype PCB solderable breadboard (pack of 5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    6-pin PCB screw terminal block connector (pack of 15)</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Jumper cables (male-to-male) (pack of 120)</t>
   </si>
   <si>
@@ -284,22 +251,13 @@
     <t xml:space="preserve">    AM-240: Rod-based Mounting Fixture</t>
   </si>
   <si>
-    <t xml:space="preserve">    Command strips</t>
-  </si>
-  <si>
     <t>Sold in packs of 12 pairs. Used for mounting hardware inside enclosure (housekeeping essentially)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Cable glands (pack of 20)</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Radiation shield</t>
   </si>
   <si>
     <t>For the Apogee ST-110 air temperature sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Southwire 3/4" aluminum conduit (100-ft length)</t>
   </si>
   <si>
     <r>
@@ -320,18 +278,12 @@
     <t>seeed studio module that can help control power to the apogee radiometer heaters</t>
   </si>
   <si>
-    <t>We had existing panels. Can find similar panels online for $50+. Note that you may need a different wattage based on your implementation</t>
-  </si>
-  <si>
     <t xml:space="preserve">    12V DC to 5V USB-C female DC step-down converter</t>
   </si>
   <si>
     <t>Takes 12 volts down to what the Mayfly can handle</t>
   </si>
   <si>
-    <t xml:space="preserve">    Spade connectors for quick battery connect (pack of 20)</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Primary wire (black)</t>
   </si>
   <si>
@@ -345,6 +297,66 @@
   </si>
   <si>
     <t>For air temperature. Analog bridge measurement</t>
+  </si>
+  <si>
+    <t>32 GB (Link is to a pack of 2 for $12.47)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3-port lever wire connectors (pack of 10)</t>
+  </si>
+  <si>
+    <t>Sold in pack of 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Compact wire splice connector quick terminal block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    EnvrioDIY grove to 3.5mm stereo jack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Prototype PCB solderable breadboard</t>
+  </si>
+  <si>
+    <t>For securing and connecting peripheral ADCs. Sold in packs of 5 for $8.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6-pin PCB screw terminal block connector</t>
+  </si>
+  <si>
+    <t>One enclosure for the data logger and one for the battery. If you decide to go with a small enough battery to fit in the same enclosure as the data logger then you don't need two of these</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Command strips package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Cable glands package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Southwire 3/4" aluminum conduit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    12V 35Ah sealed lead acid battery</t>
+  </si>
+  <si>
+    <t>This is just a basic size suggestion if you don't want to worry about sizing for a smaller battery. This should do if you get halfway-decent solar recharge</t>
+  </si>
+  <si>
+    <t>Note that this is for just 10 watts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    16 AWG extension cable for solar panel (25-ft length)</t>
+  </si>
+  <si>
+    <t>Only necessary if locating solar panel away from station, in which case you will need to measure out how much you need.</t>
+  </si>
+  <si>
+    <t>Sold in 100ft length for $103. Used for protecting soil moisture sensor cables from critters. 4 feet needed for soil sensors, but you may need more if you choose to locate solar panel away from mast and run the cable through it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Alligator Clips</t>
+  </si>
+  <si>
+    <t>These are needed to make a connection to the battery. Sold in packs of 6 for $3.99</t>
   </si>
 </sst>
 </file>
@@ -429,7 +441,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,7 +457,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -767,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4E0150-E134-1049-A012-C7D00DAA06DE}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -849,7 +860,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -912,7 +923,7 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -938,305 +949,305 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="7">
-        <v>12.65</v>
+        <v>7.98</v>
       </c>
       <c r="D10" s="7">
-        <f t="shared" ref="D10:D17" si="1">B10*C10</f>
-        <v>12.65</v>
+        <f>B10*C10</f>
+        <v>7.98</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="7">
-        <v>35</v>
+        <v>6.23</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" si="1"/>
-        <v>35</v>
+        <f t="shared" ref="D11:D18" si="1">B11*C11</f>
+        <v>6.23</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="7">
-        <v>22.98</v>
+        <v>7</v>
       </c>
       <c r="D12" s="7">
         <f t="shared" si="1"/>
-        <v>22.98</v>
+        <v>21</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="7">
-        <v>8.49</v>
+        <v>2.87</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" si="1"/>
-        <v>8.49</v>
-      </c>
-      <c r="E13" s="3" t="s">
+        <v>5.74</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="7">
-        <v>14.95</v>
+        <v>1.7</v>
       </c>
       <c r="D14" s="7">
         <f t="shared" si="1"/>
-        <v>29.9</v>
+        <v>1.7</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="7">
-        <v>12.99</v>
+        <v>14.95</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="1"/>
-        <v>12.99</v>
+        <v>29.9</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16" s="7">
-        <v>6.88</v>
+        <v>0.81</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" si="1"/>
-        <v>6.88</v>
+        <v>3.24</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" s="7">
-        <v>9.99</v>
+        <v>6.88</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" si="1"/>
+        <v>6.88</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
         <v>9.99</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="8">
-        <f>SUM(D4:D17)</f>
-        <v>356.79000000000008</v>
-      </c>
-      <c r="E18" s="5"/>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
+        <v>9.99</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="16">
+        <v>10</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="D19" s="17">
+        <f>B19*C19</f>
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="8">
+        <f>SUM(D4:D19)</f>
+        <v>316.46999999999997</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7">
-        <v>162.94999999999999</v>
-      </c>
-      <c r="D21" s="7">
-        <f>B21*C21</f>
-        <v>162.94999999999999</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" s="16">
-        <v>2.08</v>
-      </c>
-      <c r="D22" s="7">
-        <f>B22*C22</f>
-        <v>4.16</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" s="7">
-        <v>42</v>
+        <v>162.94999999999999</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" ref="D23:D32" si="2">B23*C23</f>
-        <v>84</v>
-      </c>
-      <c r="E23" s="6" t="s">
+        <f>B23*C23</f>
+        <v>325.89999999999998</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24" s="7">
-        <v>84</v>
+      <c r="C24" s="15">
+        <v>2.08</v>
       </c>
       <c r="D24" s="7">
-        <f>C24*B24</f>
-        <v>168</v>
+        <f>B24*C24</f>
+        <v>4.16</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="7">
-        <v>3.43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="2"/>
-        <v>3.43</v>
+        <f t="shared" ref="D25:D34" si="2">B25*C25</f>
+        <v>84</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="7">
-        <v>9.98</v>
+        <v>84</v>
       </c>
       <c r="D26" s="7">
-        <f t="shared" si="2"/>
-        <v>9.98</v>
+        <f>C26*B26</f>
+        <v>168</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1247,568 +1258,590 @@
         <v>1</v>
       </c>
       <c r="C27" s="7">
-        <v>7.4</v>
+        <v>3.43</v>
       </c>
       <c r="D27" s="7">
         <f t="shared" si="2"/>
-        <v>7.4</v>
+        <v>3.43</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" s="7">
-        <v>8.49</v>
+        <v>9.98</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" si="2"/>
-        <v>8.49</v>
+        <v>9.98</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="7">
-        <v>54.99</v>
+        <v>7.4</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="2"/>
-        <v>54.99</v>
+        <v>7.4</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="7">
-        <v>7.49</v>
+        <v>8.49</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="2"/>
-        <v>7.49</v>
+        <v>8.49</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="7">
-        <v>4.68</v>
+        <v>54.99</v>
       </c>
       <c r="D31" s="7">
         <f t="shared" si="2"/>
-        <v>4.68</v>
+        <v>54.99</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" s="7">
-        <v>103</v>
+        <v>7.49</v>
       </c>
       <c r="D32" s="7">
         <f t="shared" si="2"/>
-        <v>103</v>
+        <v>7.49</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="8">
-        <f>SUM(D21:D32)</f>
-        <v>618.57000000000005</v>
-      </c>
-      <c r="E33" s="5"/>
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <v>4.68</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="2"/>
+        <v>4.68</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1.03</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="2"/>
+        <v>4.12</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="8">
+        <f>SUM(D23:D34)</f>
+        <v>682.63999999999987</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7">
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="7">
         <v>7.6</v>
       </c>
-      <c r="D36" s="7">
-        <f>B36*C36</f>
+      <c r="D38" s="7">
+        <f>B38*C38</f>
         <v>7.6</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="15">
-        <v>214</v>
-      </c>
-      <c r="D37" s="7">
-        <f t="shared" ref="D37:D38" si="3">B37*C37</f>
-        <v>214</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" s="7">
-        <v>50.99</v>
-      </c>
-      <c r="D38" s="7">
-        <f t="shared" si="3"/>
-        <v>50.99</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F38" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" s="15">
-        <v>312</v>
+        <v>214</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" ref="D39:D40" si="4">B39*C39</f>
-        <v>312</v>
+        <f t="shared" ref="D39:D40" si="3">B39*C39</f>
+        <v>214</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F39" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="7">
+        <v>86.99</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="3"/>
+        <v>86.99</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="15">
+        <v>312</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" ref="D41:D42" si="4">B41*C41</f>
+        <v>312</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="15">
         <v>8.99</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D42" s="7">
         <f t="shared" si="4"/>
         <v>8.99</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="16">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="D41" s="7">
-        <f t="shared" ref="D41" si="5">B41*C41</f>
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="7">
-        <v>7.54</v>
-      </c>
-      <c r="D42" s="7">
-        <f>B42*C42</f>
-        <v>7.54</v>
-      </c>
       <c r="E42" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" s="7">
-        <v>6.63</v>
+        <v>7.54</v>
       </c>
       <c r="D43" s="7">
         <f>B43*C43</f>
+        <v>7.54</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7">
         <v>6.63</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="D44" s="7">
+        <f>B44*C44</f>
+        <v>6.63</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="15">
+        <v>15.5</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" ref="D45:D46" si="5">B45*C45</f>
+        <v>15.5</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" s="15">
+        <v>0.67</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="5"/>
+        <v>1.34</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8">
-        <f>SUM(D36:D43)</f>
-        <v>611.93999999999994</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="B47" s="2"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8">
+        <f>SUM(D38:D46)</f>
+        <v>660.58999999999992</v>
+      </c>
+      <c r="E47" s="5"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>22</v>
       </c>
-      <c r="B47">
+      <c r="B50">
         <v>3</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C50" s="7">
         <v>258</v>
       </c>
-      <c r="D47" s="7">
-        <f t="shared" ref="D47:D53" si="6">B47*C47</f>
+      <c r="D50" s="7">
+        <f t="shared" ref="D50:D55" si="6">B50*C50</f>
         <v>774</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" s="7">
+      <c r="E50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="7">
         <v>134</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D51" s="7">
         <f t="shared" si="6"/>
         <v>134</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="17">
-        <v>10</v>
-      </c>
-      <c r="C49" s="18">
-        <v>0.59</v>
-      </c>
-      <c r="D49" s="18">
-        <f t="shared" si="6"/>
-        <v>5.8999999999999995</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" s="7">
+      <c r="E51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" s="7">
         <v>599</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D52" s="7">
         <f t="shared" si="6"/>
         <v>599</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" s="7">
+      <c r="E52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" s="7">
         <v>599</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D53" s="7">
         <f t="shared" si="6"/>
         <v>599</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" s="7">
+      <c r="E53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="7">
         <v>663</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D54" s="7">
         <f t="shared" si="6"/>
         <v>663</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" s="7">
+      <c r="E54" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" s="7">
         <v>85</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D55" s="7">
         <f t="shared" si="6"/>
         <v>85</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8">
-        <f>SUM(D47:D53)</f>
-        <v>2859.9</v>
-      </c>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E55" s="1"/>
+      <c r="E55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E56" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8">
+        <f>SUM(D50:D55)</f>
+        <v>2854</v>
+      </c>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" s="15">
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" s="7">
         <v>926.4</v>
       </c>
-      <c r="D57" s="7">
-        <f t="shared" ref="D57:D58" si="7">B57*C57</f>
+      <c r="D59" s="7">
+        <f t="shared" ref="D59:D60" si="7">B59*C59</f>
         <v>926.4</v>
       </c>
-      <c r="E57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" s="15">
+      <c r="E59" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" s="7">
         <v>162.24</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D60" s="7">
         <f t="shared" si="7"/>
         <v>162.24</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="E60" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8">
-        <f>SUM(D57:D58)</f>
+      <c r="B61" s="2"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8">
+        <f>SUM(D59:D60)</f>
         <v>1088.6399999999999</v>
       </c>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B61" s="10"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13">
-        <f>SUM(D18,D33,D44,D54,D59)</f>
-        <v>5535.84</v>
-      </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="11"/>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
@@ -1817,54 +1850,76 @@
       <c r="D62" s="8"/>
       <c r="E62" s="5"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13">
+        <f>SUM(D20,D35,D47,D56,D61)</f>
+        <v>5602.34</v>
+      </c>
+      <c r="E63" s="14"/>
+      <c r="F63" s="11"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="5"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{265C8903-4AEC-DE44-B1F0-7DCFD4E09549}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{D7F77966-9390-464E-8627-399015801D2B}"/>
-    <hyperlink ref="E47" r:id="rId3" xr:uid="{753A6B9C-278C-CF4C-84C9-5C0074671CCB}"/>
+    <hyperlink ref="E50" r:id="rId3" xr:uid="{753A6B9C-278C-CF4C-84C9-5C0074671CCB}"/>
     <hyperlink ref="E7" r:id="rId4" xr:uid="{ABA722A5-FBD9-5648-907E-EA5124EDD3C7}"/>
     <hyperlink ref="E4" r:id="rId5" xr:uid="{E86130E0-C24B-4999-BA56-A93018628621}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{5EBE1F0E-BB73-4E1F-930A-245A6D604944}"/>
     <hyperlink ref="E9" r:id="rId7" xr:uid="{C7BB61A7-0012-4FEB-A37B-5F84C8414755}"/>
-    <hyperlink ref="E10" r:id="rId8" xr:uid="{61052F43-0BB2-4FEC-A7B9-AE85917C5F01}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{50D931CC-3B6E-42C8-808A-560D3BAA8C9B}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{932D3A23-2C68-463E-B52B-0FE8F78ACCDF}"/>
-    <hyperlink ref="E21" r:id="rId11" xr:uid="{32EB265C-265F-4027-B26C-1FFB49E4714D}"/>
-    <hyperlink ref="E22" r:id="rId12" xr:uid="{53B2F0F9-A580-4861-BD66-85ABAE1CCBAE}"/>
-    <hyperlink ref="E37" r:id="rId13" xr:uid="{3428F4BB-AED8-421F-B9A7-5D46EADA6ECE}"/>
-    <hyperlink ref="E38" r:id="rId14" xr:uid="{2432909A-C9F9-4DD3-9078-1E73DD7EF56E}"/>
-    <hyperlink ref="E39" r:id="rId15" xr:uid="{82B713F0-4D84-41F4-AC71-D5CC1FBBC40D}"/>
-    <hyperlink ref="E48" r:id="rId16" xr:uid="{FFFB96A5-D75D-44BD-A842-0A4287651080}"/>
-    <hyperlink ref="E52" r:id="rId17" xr:uid="{F23935C7-47F1-4B40-BADF-D879792EF9DE}"/>
-    <hyperlink ref="E50" r:id="rId18" xr:uid="{1D128B7C-5EF3-484D-8C28-188F278102B0}"/>
-    <hyperlink ref="E51" r:id="rId19" xr:uid="{3D0664EC-1A4C-4C99-B561-BD442A1E3D41}"/>
-    <hyperlink ref="E57" r:id="rId20" xr:uid="{2BB7E1ED-B659-4AC0-9D56-035CFD2D6858}"/>
-    <hyperlink ref="E58" r:id="rId21" xr:uid="{B7BD41D6-7DEE-43DB-95AF-95E2AAD32A07}"/>
-    <hyperlink ref="E23" r:id="rId22" xr:uid="{FC965190-7076-4E27-B4A0-310608B333A5}"/>
-    <hyperlink ref="E25" r:id="rId23" xr:uid="{4584B495-BC8B-4A56-8488-938C8F973486}"/>
-    <hyperlink ref="E27" r:id="rId24" xr:uid="{4CFD3088-B3B3-4D6F-871E-6C39CB72D32C}"/>
-    <hyperlink ref="E32" r:id="rId25" xr:uid="{6F13B64E-341D-4630-9A15-274D20E0D01A}"/>
-    <hyperlink ref="E28" r:id="rId26" xr:uid="{D339FF2C-D50A-4B5C-95DB-4E5B1D2FC78C}"/>
-    <hyperlink ref="E13" r:id="rId27" xr:uid="{AA0AA21E-916F-4519-ACCE-D922984B922D}"/>
-    <hyperlink ref="E14" r:id="rId28" xr:uid="{2B688FC6-3D9D-41FE-A949-09240AFE614E}"/>
-    <hyperlink ref="E17" r:id="rId29" xr:uid="{2B9323DA-1AF6-4F75-A730-CBCDA0051360}"/>
-    <hyperlink ref="E15" r:id="rId30" xr:uid="{522CDC08-C296-4B19-AF41-6EE0D735451A}"/>
-    <hyperlink ref="E16" r:id="rId31" xr:uid="{E2623B61-A04B-4912-8A60-A55C2FA9936D}"/>
-    <hyperlink ref="E30" r:id="rId32" xr:uid="{319EF437-6976-40FE-A61A-7768248D5FF7}"/>
-    <hyperlink ref="E31" r:id="rId33" xr:uid="{DECD7A00-C6E8-47A8-933C-60A59B1E6C6D}"/>
-    <hyperlink ref="E41" r:id="rId34" xr:uid="{A6EA964E-6FA5-469E-B251-371A48BA96A7}"/>
-    <hyperlink ref="E49" r:id="rId35" xr:uid="{B32FBE35-C99A-5D4E-BADE-D0C8CE13F03D}"/>
-    <hyperlink ref="E24" r:id="rId36" xr:uid="{31C963D8-D48F-4399-877A-80C6A1FDF2DF}"/>
-    <hyperlink ref="E26" r:id="rId37" xr:uid="{7523E5F4-A5D0-44CE-AE58-6061FDA55C5D}"/>
-    <hyperlink ref="E29" r:id="rId38" xr:uid="{890A06C2-9E75-444B-9543-24297DCBB4AD}"/>
-    <hyperlink ref="E36" r:id="rId39" xr:uid="{4DDA532A-4A95-46E4-92F8-D7CCB428C688}"/>
-    <hyperlink ref="E40" r:id="rId40" xr:uid="{682D7A7D-4104-422C-BB39-F21DDD14432B}"/>
-    <hyperlink ref="E42" r:id="rId41" xr:uid="{238EDCF7-43A6-4292-8373-67DD8FF70F05}"/>
-    <hyperlink ref="E43" r:id="rId42" xr:uid="{FF5C2C53-4B42-4969-962D-9162EFCA93B4}"/>
-    <hyperlink ref="E53" r:id="rId43" xr:uid="{1FC80352-32BF-497E-B86C-77366F41EDD7}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{61052F43-0BB2-4FEC-A7B9-AE85917C5F01}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{50D931CC-3B6E-42C8-808A-560D3BAA8C9B}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{932D3A23-2C68-463E-B52B-0FE8F78ACCDF}"/>
+    <hyperlink ref="E23" r:id="rId11" xr:uid="{32EB265C-265F-4027-B26C-1FFB49E4714D}"/>
+    <hyperlink ref="E24" r:id="rId12" xr:uid="{53B2F0F9-A580-4861-BD66-85ABAE1CCBAE}"/>
+    <hyperlink ref="E39" r:id="rId13" xr:uid="{3428F4BB-AED8-421F-B9A7-5D46EADA6ECE}"/>
+    <hyperlink ref="E41" r:id="rId14" xr:uid="{82B713F0-4D84-41F4-AC71-D5CC1FBBC40D}"/>
+    <hyperlink ref="E51" r:id="rId15" xr:uid="{FFFB96A5-D75D-44BD-A842-0A4287651080}"/>
+    <hyperlink ref="E54" r:id="rId16" xr:uid="{F23935C7-47F1-4B40-BADF-D879792EF9DE}"/>
+    <hyperlink ref="E52" r:id="rId17" xr:uid="{1D128B7C-5EF3-484D-8C28-188F278102B0}"/>
+    <hyperlink ref="E53" r:id="rId18" xr:uid="{3D0664EC-1A4C-4C99-B561-BD442A1E3D41}"/>
+    <hyperlink ref="E59" r:id="rId19" xr:uid="{2BB7E1ED-B659-4AC0-9D56-035CFD2D6858}"/>
+    <hyperlink ref="E60" r:id="rId20" xr:uid="{B7BD41D6-7DEE-43DB-95AF-95E2AAD32A07}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{FC965190-7076-4E27-B4A0-310608B333A5}"/>
+    <hyperlink ref="E27" r:id="rId22" xr:uid="{4584B495-BC8B-4A56-8488-938C8F973486}"/>
+    <hyperlink ref="E29" r:id="rId23" xr:uid="{4CFD3088-B3B3-4D6F-871E-6C39CB72D32C}"/>
+    <hyperlink ref="E34" r:id="rId24" xr:uid="{6F13B64E-341D-4630-9A15-274D20E0D01A}"/>
+    <hyperlink ref="E30" r:id="rId25" xr:uid="{D339FF2C-D50A-4B5C-95DB-4E5B1D2FC78C}"/>
+    <hyperlink ref="E14" r:id="rId26" xr:uid="{AA0AA21E-916F-4519-ACCE-D922984B922D}"/>
+    <hyperlink ref="E15" r:id="rId27" xr:uid="{2B688FC6-3D9D-41FE-A949-09240AFE614E}"/>
+    <hyperlink ref="E18" r:id="rId28" xr:uid="{2B9323DA-1AF6-4F75-A730-CBCDA0051360}"/>
+    <hyperlink ref="E16" r:id="rId29" xr:uid="{522CDC08-C296-4B19-AF41-6EE0D735451A}"/>
+    <hyperlink ref="E17" r:id="rId30" xr:uid="{E2623B61-A04B-4912-8A60-A55C2FA9936D}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{319EF437-6976-40FE-A61A-7768248D5FF7}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{DECD7A00-C6E8-47A8-933C-60A59B1E6C6D}"/>
+    <hyperlink ref="E19" r:id="rId33" xr:uid="{B32FBE35-C99A-5D4E-BADE-D0C8CE13F03D}"/>
+    <hyperlink ref="E26" r:id="rId34" xr:uid="{31C963D8-D48F-4399-877A-80C6A1FDF2DF}"/>
+    <hyperlink ref="E28" r:id="rId35" xr:uid="{7523E5F4-A5D0-44CE-AE58-6061FDA55C5D}"/>
+    <hyperlink ref="E31" r:id="rId36" xr:uid="{890A06C2-9E75-444B-9543-24297DCBB4AD}"/>
+    <hyperlink ref="E38" r:id="rId37" xr:uid="{4DDA532A-4A95-46E4-92F8-D7CCB428C688}"/>
+    <hyperlink ref="E42" r:id="rId38" xr:uid="{682D7A7D-4104-422C-BB39-F21DDD14432B}"/>
+    <hyperlink ref="E43" r:id="rId39" xr:uid="{238EDCF7-43A6-4292-8373-67DD8FF70F05}"/>
+    <hyperlink ref="E44" r:id="rId40" xr:uid="{FF5C2C53-4B42-4969-962D-9162EFCA93B4}"/>
+    <hyperlink ref="E55" r:id="rId41" xr:uid="{1FC80352-32BF-497E-B86C-77366F41EDD7}"/>
+    <hyperlink ref="E10" r:id="rId42" xr:uid="{A03145A4-2207-4DD5-94A8-E5713A210DA9}"/>
+    <hyperlink ref="E40" r:id="rId43" xr:uid="{34147571-0194-4182-AFAD-DBC668CB6B0D}"/>
+    <hyperlink ref="E45" r:id="rId44" xr:uid="{64150BBB-D3C0-4919-9E5D-46A9DB722037}"/>
+    <hyperlink ref="E46" r:id="rId45" xr:uid="{0F168994-B5FA-452E-892C-A2E8F5D9AAFD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>